<commit_message>
Extracted Details From CSVs to Dicts
</commit_message>
<xml_diff>
--- a/datasets/TimSchedLecturers.xlsx
+++ b/datasets/TimSchedLecturers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djmck\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software Projects\ML Projects\Timetable Scheduling Algorithm\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,9 +35,6 @@
     <t>Department</t>
   </si>
   <si>
-    <t xml:space="preserve"> Status</t>
-  </si>
-  <si>
     <t>Maximum Units</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,249 +528,249 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <v>18</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3">
         <v>21</v>
       </c>
       <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
       </c>
       <c r="E4">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
       </c>
       <c r="E5">
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
       </c>
       <c r="E8">
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
       </c>
       <c r="E9">
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10">
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
       </c>
       <c r="E11">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>